<commit_message>
Back para modificar BD
</commit_message>
<xml_diff>
--- a/backendRUVI1/gestionPacientes/PRESTACIONES_CAUSAS.xlsx
+++ b/backendRUVI1/gestionPacientes/PRESTACIONES_CAUSAS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAX\Desktop\proyectojango\copia practica\RUVI1Pingeso\backendRUVI1\gestionPacientes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAX\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFEE18F-48C1-44BA-A770-9530D6B6A143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274D3914-1249-4314-95B3-4163298FCF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6FFEF54C-297C-4852-B3BA-84F23CE229AB}"/>
   </bookViews>
@@ -29,20 +29,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="86">
   <si>
     <t>ECOCARDIO TT</t>
   </si>
@@ -297,13 +289,16 @@
   </si>
   <si>
     <t>TERAPIA INTRAHOSPITALARIA</t>
+  </si>
+  <si>
+    <t>Prestacion de prueba</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,6 +327,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -353,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -367,6 +370,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1060,10 +1064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE9988D7-C80E-4AFE-9A7B-880620EBB098}">
-  <dimension ref="A1:B82"/>
+  <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1584,7 +1588,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>40</v>
       </c>
@@ -1592,7 +1596,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>74</v>
       </c>
@@ -1600,7 +1604,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>72</v>
       </c>
@@ -1608,7 +1612,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>75</v>
       </c>
@@ -1616,7 +1620,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>76</v>
       </c>
@@ -1624,7 +1628,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>61</v>
       </c>
@@ -1632,7 +1636,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
         <v>67</v>
       </c>
@@ -1640,7 +1644,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>53</v>
       </c>
@@ -1648,7 +1652,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>66</v>
       </c>
@@ -1656,7 +1660,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
         <v>55</v>
       </c>
@@ -1664,7 +1668,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
         <v>62</v>
       </c>
@@ -1672,7 +1676,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
         <v>64</v>
       </c>
@@ -1680,7 +1684,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
         <v>77</v>
       </c>
@@ -1688,7 +1692,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>63</v>
       </c>
@@ -1696,7 +1700,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
         <v>65</v>
       </c>
@@ -1704,13 +1708,14 @@
         <v>59</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="C80" s="5"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
@@ -1721,7 +1726,12 @@
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A82" s="2"/>
+      <c r="A82" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:B57" xr:uid="{DE9988D7-C80E-4AFE-9A7B-880620EBB098}">
@@ -1730,5 +1740,6 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Eliminado de usuarios, filtro servicios conectado, fix errores menores
</commit_message>
<xml_diff>
--- a/backendRUVI1/gestionPacientes/PRESTACIONES_CAUSAS.xlsx
+++ b/backendRUVI1/gestionPacientes/PRESTACIONES_CAUSAS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAX\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ccbd8c86b1c6efc9/Escritorio/Pingeso/RUVI1Pingeso/backendRUVI1/gestionPacientes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274D3914-1249-4314-95B3-4163298FCF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{274D3914-1249-4314-95B3-4163298FCF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06E5EC20-E190-4242-9C0E-5403817BB5C5}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6FFEF54C-297C-4852-B3BA-84F23CE229AB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6FFEF54C-297C-4852-B3BA-84F23CE229AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Prestaciones" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="85">
   <si>
     <t>ECOCARDIO TT</t>
   </si>
@@ -289,9 +289,6 @@
   </si>
   <si>
     <t>TERAPIA INTRAHOSPITALARIA</t>
-  </si>
-  <si>
-    <t>Prestacion de prueba</t>
   </si>
 </sst>
 </file>
@@ -1066,17 +1063,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE9988D7-C80E-4AFE-9A7B-880620EBB098}">
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.26953125" customWidth="1"/>
+    <col min="1" max="1" width="33.21875" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1084,7 +1081,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1092,7 +1089,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1100,7 +1097,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1108,7 +1105,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1116,7 +1113,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1124,7 +1121,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1132,7 +1129,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1140,7 +1137,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -1148,7 +1145,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -1156,7 +1153,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -1164,7 +1161,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -1172,7 +1169,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -1180,7 +1177,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -1188,7 +1185,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
@@ -1196,7 +1193,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
@@ -1204,7 +1201,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
@@ -1212,7 +1209,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
@@ -1220,7 +1217,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1228,7 +1225,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>80</v>
       </c>
@@ -1236,7 +1233,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
@@ -1244,7 +1241,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
@@ -1252,7 +1249,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
@@ -1260,7 +1257,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>27</v>
       </c>
@@ -1268,7 +1265,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
@@ -1276,7 +1273,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>29</v>
       </c>
@@ -1284,7 +1281,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
@@ -1292,7 +1289,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>31</v>
       </c>
@@ -1300,7 +1297,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>32</v>
       </c>
@@ -1308,7 +1305,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>33</v>
       </c>
@@ -1316,7 +1313,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>34</v>
       </c>
@@ -1324,7 +1321,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>35</v>
       </c>
@@ -1332,7 +1329,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>36</v>
       </c>
@@ -1340,7 +1337,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>37</v>
       </c>
@@ -1348,7 +1345,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -1356,7 +1353,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>41</v>
       </c>
@@ -1364,7 +1361,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>42</v>
       </c>
@@ -1372,7 +1369,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>43</v>
       </c>
@@ -1380,7 +1377,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>44</v>
       </c>
@@ -1388,7 +1385,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>45</v>
       </c>
@@ -1396,7 +1393,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>46</v>
       </c>
@@ -1404,7 +1401,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>47</v>
       </c>
@@ -1412,7 +1409,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>48</v>
       </c>
@@ -1420,7 +1417,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>49</v>
       </c>
@@ -1428,7 +1425,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>50</v>
       </c>
@@ -1436,7 +1433,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>51</v>
       </c>
@@ -1444,7 +1441,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>52</v>
       </c>
@@ -1452,7 +1449,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>54</v>
       </c>
@@ -1460,7 +1457,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>56</v>
       </c>
@@ -1468,7 +1465,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>78</v>
       </c>
@@ -1476,7 +1473,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>81</v>
       </c>
@@ -1484,7 +1481,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>6</v>
       </c>
@@ -1492,7 +1489,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>71</v>
       </c>
@@ -1500,7 +1497,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>15</v>
       </c>
@@ -1508,7 +1505,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>16</v>
       </c>
@@ -1516,7 +1513,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>20</v>
       </c>
@@ -1524,7 +1521,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>70</v>
       </c>
@@ -1532,7 +1529,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>23</v>
       </c>
@@ -1540,7 +1537,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>69</v>
       </c>
@@ -1548,7 +1545,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>68</v>
       </c>
@@ -1556,7 +1553,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>60</v>
       </c>
@@ -1564,7 +1561,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>79</v>
       </c>
@@ -1572,7 +1569,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>73</v>
       </c>
@@ -1580,7 +1577,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>38</v>
       </c>
@@ -1588,7 +1585,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>40</v>
       </c>
@@ -1596,7 +1593,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>74</v>
       </c>
@@ -1604,7 +1601,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>72</v>
       </c>
@@ -1612,7 +1609,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>75</v>
       </c>
@@ -1620,7 +1617,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>76</v>
       </c>
@@ -1628,7 +1625,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>61</v>
       </c>
@@ -1636,7 +1633,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>67</v>
       </c>
@@ -1644,7 +1641,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>53</v>
       </c>
@@ -1652,7 +1649,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>66</v>
       </c>
@@ -1660,7 +1657,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>55</v>
       </c>
@@ -1668,7 +1665,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>62</v>
       </c>
@@ -1676,7 +1673,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>64</v>
       </c>
@@ -1684,7 +1681,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>77</v>
       </c>
@@ -1692,7 +1689,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>63</v>
       </c>
@@ -1700,7 +1697,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>65</v>
       </c>
@@ -1708,7 +1705,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>82</v>
       </c>
@@ -1717,7 +1714,7 @@
       </c>
       <c r="C80" s="5"/>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>84</v>
       </c>
@@ -1725,13 +1722,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A82" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>59</v>
-      </c>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" s="2"/>
+      <c r="B82" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:B57" xr:uid="{DE9988D7-C80E-4AFE-9A7B-880620EBB098}">

</xml_diff>

<commit_message>
Filtro servicios HEGC-subida archivos
</commit_message>
<xml_diff>
--- a/backendRUVI1/gestionPacientes/PRESTACIONES_CAUSAS.xlsx
+++ b/backendRUVI1/gestionPacientes/PRESTACIONES_CAUSAS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ccbd8c86b1c6efc9/Escritorio/Pingeso/RUVI1Pingeso/backendRUVI1/gestionPacientes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAX\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{274D3914-1249-4314-95B3-4163298FCF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06E5EC20-E190-4242-9C0E-5403817BB5C5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25212E0-D6E9-4C25-B6D0-B37CEDA2A4D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6FFEF54C-297C-4852-B3BA-84F23CE229AB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6FFEF54C-297C-4852-B3BA-84F23CE229AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Prestaciones" sheetId="3" r:id="rId1"/>
@@ -1061,19 +1061,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE9988D7-C80E-4AFE-9A7B-880620EBB098}">
-  <dimension ref="A1:C82"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82:XFD82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.21875" customWidth="1"/>
+    <col min="1" max="1" width="33.26953125" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>80</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>27</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>29</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>31</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>32</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>33</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>34</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>35</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>36</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>37</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>41</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>42</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>43</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>44</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>45</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>46</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>47</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>48</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>49</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>50</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>51</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>52</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>54</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>56</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>78</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>81</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>6</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>71</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>15</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>16</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>20</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>70</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>23</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
         <v>69</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>68</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>60</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>79</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>73</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>38</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>40</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>74</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>72</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>75</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>76</v>
       </c>
@@ -1625,7 +1625,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>61</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
         <v>67</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>53</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>66</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
         <v>55</v>
       </c>
@@ -1665,15 +1665,16 @@
         <v>59</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D75" s="5"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
         <v>64</v>
       </c>
@@ -1681,7 +1682,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
         <v>77</v>
       </c>
@@ -1689,7 +1690,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>63</v>
       </c>
@@ -1697,7 +1698,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
         <v>65</v>
       </c>
@@ -1705,7 +1706,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>82</v>
       </c>
@@ -1714,7 +1715,7 @@
       </c>
       <c r="C80" s="5"/>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
         <v>84</v>
       </c>
@@ -1722,7 +1723,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" s="2"/>
       <c r="B82" s="3"/>
     </row>

</xml_diff>